<commit_message>
update mhc_ligands benchmarking for non-text-shifting methods
</commit_message>
<xml_diff>
--- a/benchmarking/mhc-ligands-benchmarking.xlsx
+++ b/benchmarking/mhc-ligands-benchmarking.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">N/A</t>
   </si>
   <si>
-    <t xml:space="preserve">NmerMatch</t>
+    <t xml:space="preserve">NmerMatch (J Greenbaum)</t>
   </si>
   <si>
     <t xml:space="preserve">Horspool algorithm</t>
@@ -193,7 +193,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -232,48 +232,48 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>37.839</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0.071</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>37.91</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1" t="n">
+      <c r="B2" s="0" t="n">
+        <v>39.617</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>39.697</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>55.0901165008545</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>0.00350117683410644</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>13.75</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>68.844</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="n">
+      <c r="B3" s="0" t="n">
+        <v>53.716</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.0055389404296875</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>12.319</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>66.041</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -373,22 +373,22 @@
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>1.30349087715149</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>6.657</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>7.961</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1" t="n">
+      <c r="B8" s="0" t="n">
+        <v>1.265</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>11.29</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>12.555</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>98.304</v>
       </c>
     </row>
@@ -396,22 +396,22 @@
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>0.245501756668091</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>4.656</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>4.901</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="1" t="n">
+      <c r="B9" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>5.011</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>5.262</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>1.495</v>
       </c>
     </row>
@@ -419,22 +419,22 @@
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>2.35403919219971</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>0.532</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>2.886</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="1" t="n">
+      <c r="B10" s="0" t="n">
+        <v>2.645</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.497</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>3.142</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>